<commit_message>
Updated project description and BOM
</commit_message>
<xml_diff>
--- a/Project Planning/Plotter-BOM.xlsx
+++ b/Project Planning/Plotter-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Plotting\Github\CNC-Plotter\Project Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9E376A-E02F-42E5-8C57-B096996F142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C06610A-28C7-4D25-974A-5EB21AEA4D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{EBA329A8-BC4F-4D43-8656-7391979E98BE}"/>
+    <workbookView xWindow="5835" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{EBA329A8-BC4F-4D43-8656-7391979E98BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Item</t>
   </si>
@@ -86,9 +86,6 @@
     <t>mg90s Micro Servo</t>
   </si>
   <si>
-    <t>MDF Board</t>
-  </si>
-  <si>
     <t>17HS15-1504S-X1</t>
   </si>
   <si>
@@ -99,16 +96,54 @@
   </si>
   <si>
     <t>DRV8825</t>
+  </si>
+  <si>
+    <t>CNC Shield V3</t>
+  </si>
+  <si>
+    <t>Mean Well LRS-150-24</t>
+  </si>
+  <si>
+    <t>https://8020.net/20-2040.html</t>
+  </si>
+  <si>
+    <t>https://8020.net/20-2020.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDF Board </t>
+  </si>
+  <si>
+    <t>https://limobearing.com/mgn12c-mgn12h-mini-linear-sliding-rail</t>
+  </si>
+  <si>
+    <t>https://limobearing.com/mgn7h-mgn7c-miniature-linear-ball-rail</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-17-bipolar-45ncm-63-74oz-in-1-5a-42x42x39mm-4-wires-w-1m-pin-connector-17hs15-1504s-x1</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-17-bipolar-1-8deg-65ncm-92oz-in-2-1a-3-36v-42x42x60mm-4-wires-17hs24-2104s</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/lrs-150-24-mean-well-150w-24vdc-6-5a-115-230vac-enclosed-switching-power-supply-lrs-150-24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,14 +166,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -159,8 +196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B5AFC2A-95CA-42C6-BDE3-6D82C10D080B}" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17" xr:uid="{2B5AFC2A-95CA-42C6-BDE3-6D82C10D080B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B5AFC2A-95CA-42C6-BDE3-6D82C10D080B}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0">
+  <autoFilter ref="A1:E19" xr:uid="{2B5AFC2A-95CA-42C6-BDE3-6D82C10D080B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AE1966D0-3DF5-4ABC-8CCB-6FB1050990C9}" name="Item"/>
     <tableColumn id="2" xr3:uid="{4891D177-A691-41D8-85A7-67D5A91E985E}" name="Quantity"/>
@@ -491,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4559454-B297-4D28-AF0B-F4923CFCDEBE}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,9 +563,15 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>38.479999999999997</v>
+      </c>
       <c r="D2">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+        <v>38.479999999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,9 +581,15 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>17.14</v>
+      </c>
       <c r="D3">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+        <v>34.28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -562,7 +611,7 @@
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
@@ -574,7 +623,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
@@ -586,7 +635,7 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
@@ -598,7 +647,7 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
@@ -610,9 +659,15 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="D9" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="C9">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="D9">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -622,9 +677,15 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="C10">
+        <v>16.27</v>
+      </c>
+      <c r="D10">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>16.27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -634,9 +695,15 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="C11">
+        <v>6.81</v>
+      </c>
+      <c r="D11">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>6.81</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -646,75 +713,127 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="C14">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="D14">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="C15">
+        <v>13.24</v>
+      </c>
+      <c r="D15">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>13.24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="D17" s="1">
-        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
-        <v>0</v>
+      <c r="D17">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>11.48</v>
+      </c>
+      <c r="D19">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Cost Per Item]]</f>
+        <v>11.48</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>SUM(Table1[Total Cost])</f>
+        <v>167.98999999999998</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{B2B85C19-172F-4C53-BFE1-1AC1A6ED2E62}"/>
+    <hyperlink ref="E19" r:id="rId2" xr:uid="{3BECA83F-6E6D-470F-8302-A85F95BDB81D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>